<commit_message>
error_method: Narrow or Cramer   + output options
</commit_message>
<xml_diff>
--- a/BGT.xlsx
+++ b/BGT.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CH23"/>
+  <dimension ref="A1:CH26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -696,7 +696,7 @@
       </c>
       <c r="BA1" s="1" t="inlineStr">
         <is>
-          <t>LWP758</t>
+          <t>LWP761</t>
         </is>
       </c>
       <c r="BB1" s="1" t="inlineStr">
@@ -9928,432 +9928,1728 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>LWP755</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>1.003878e+01</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>1.752502e+00</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>0.000000e+00</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>1.538832e+01</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>6.882262e+00</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>3.892974e+00</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>1.066977e+01</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>1.567930e+01</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>1.350907e+01</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>0.000000e+00</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>0.000000e+00</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>7.227516e+00</t>
+        </is>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>1.352367e+01</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>4.059606e+00</t>
+        </is>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>6.755814e+00</t>
+        </is>
+      </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>0.000000e+00</t>
+        </is>
+      </c>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>0.000000e+00</t>
+        </is>
+      </c>
+      <c r="V23" t="inlineStr">
+        <is>
+          <t>0.000000e+00</t>
+        </is>
+      </c>
+      <c r="W23" t="inlineStr">
+        <is>
+          <t>1.178902e+01</t>
+        </is>
+      </c>
+      <c r="X23" t="inlineStr">
+        <is>
+          <t>1.758328e+01</t>
+        </is>
+      </c>
+      <c r="Y23" t="inlineStr">
+        <is>
+          <t>1.064879e+01</t>
+        </is>
+      </c>
+      <c r="Z23" t="inlineStr">
+        <is>
+          <t>2.918837e+01</t>
+        </is>
+      </c>
+      <c r="AA23" t="inlineStr">
+        <is>
+          <t>LWP755</t>
+        </is>
+      </c>
+      <c r="AB23" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="AC23" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="AD23" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AE23" t="inlineStr">
+        <is>
+          <t>3.596999e+00</t>
+        </is>
+      </c>
+      <c r="AF23" t="inlineStr">
+        <is>
+          <t>2.269048e+00</t>
+        </is>
+      </c>
+      <c r="AG23" t="inlineStr">
+        <is>
+          <t>3.933038e+00</t>
+        </is>
+      </c>
+      <c r="AH23" t="inlineStr">
+        <is>
+          <t>2.341836e+00</t>
+        </is>
+      </c>
+      <c r="AI23" t="inlineStr">
+        <is>
+          <t>4.324382e+00</t>
+        </is>
+      </c>
+      <c r="AJ23" t="inlineStr">
+        <is>
+          <t>3.684784e+00</t>
+        </is>
+      </c>
+      <c r="AK23" t="inlineStr">
+        <is>
+          <t>8.499564e+00</t>
+        </is>
+      </c>
+      <c r="AL23" t="inlineStr">
+        <is>
+          <t>8.848250e+00</t>
+        </is>
+      </c>
+      <c r="AM23" t="inlineStr">
+        <is>
+          <t>5.056651e+00</t>
+        </is>
+      </c>
+      <c r="AN23" t="inlineStr">
+        <is>
+          <t>2.358123e+00</t>
+        </is>
+      </c>
+      <c r="AO23" t="inlineStr">
+        <is>
+          <t>5.920429e+00</t>
+        </is>
+      </c>
+      <c r="AP23" t="inlineStr">
+        <is>
+          <t>4.556646e+00</t>
+        </is>
+      </c>
+      <c r="AQ23" t="inlineStr">
+        <is>
+          <t>4.161243e+00</t>
+        </is>
+      </c>
+      <c r="AR23" t="inlineStr">
+        <is>
+          <t>5.077954e+00</t>
+        </is>
+      </c>
+      <c r="AS23" t="inlineStr">
+        <is>
+          <t>3.183925e+00</t>
+        </is>
+      </c>
+      <c r="AT23" t="inlineStr">
+        <is>
+          <t>9.124146e-01</t>
+        </is>
+      </c>
+      <c r="AU23" t="inlineStr">
+        <is>
+          <t>5.337463e-01</t>
+        </is>
+      </c>
+      <c r="AV23" t="inlineStr">
+        <is>
+          <t>2.773363e+00</t>
+        </is>
+      </c>
+      <c r="AW23" t="inlineStr">
+        <is>
+          <t>5.662991e+00</t>
+        </is>
+      </c>
+      <c r="AX23" t="inlineStr">
+        <is>
+          <t>2.254865e+00</t>
+        </is>
+      </c>
+      <c r="AY23" t="inlineStr">
+        <is>
+          <t>1.021641e+00</t>
+        </is>
+      </c>
+      <c r="AZ23" t="inlineStr">
+        <is>
+          <t>7.919957e+00</t>
+        </is>
+      </c>
+      <c r="BA23" t="inlineStr">
+        <is>
+          <t>LWP755</t>
+        </is>
+      </c>
+      <c r="BB23" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="BC23" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="BD23" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BE23" t="inlineStr">
+        <is>
+          <t>1.220547e+00</t>
+        </is>
+      </c>
+      <c r="BF23" t="inlineStr">
+        <is>
+          <t>2.694449e+01</t>
+        </is>
+      </c>
+      <c r="BG23" t="inlineStr">
+        <is>
+          <t>9.171451e+01</t>
+        </is>
+      </c>
+      <c r="BH23" t="inlineStr">
+        <is>
+          <t>0.000000e+00</t>
+        </is>
+      </c>
+      <c r="BI23" t="inlineStr">
+        <is>
+          <t>4.966743e-02</t>
+        </is>
+      </c>
+      <c r="BJ23" t="inlineStr">
+        <is>
+          <t>6.347656e+00</t>
+        </is>
+      </c>
+      <c r="BK23" t="inlineStr">
+        <is>
+          <t>6.424181e+00</t>
+        </is>
+      </c>
+      <c r="BL23" t="inlineStr">
+        <is>
+          <t>7.841013e+00</t>
+        </is>
+      </c>
+      <c r="BM23" t="inlineStr">
+        <is>
+          <t>7.841013e+00</t>
+        </is>
+      </c>
+      <c r="BN23" t="inlineStr">
+        <is>
+          <t>1.234827e-02</t>
+        </is>
+      </c>
+      <c r="BO23" t="inlineStr">
+        <is>
+          <t>1.300703e-02</t>
+        </is>
+      </c>
+      <c r="BP23" t="inlineStr">
+        <is>
+          <t>4.674834e+00</t>
+        </is>
+      </c>
+      <c r="BQ23" t="inlineStr">
+        <is>
+          <t>6.010892e+01</t>
+        </is>
+      </c>
+      <c r="BR23" t="inlineStr">
+        <is>
+          <t>8.740408e+01</t>
+        </is>
+      </c>
+      <c r="BS23" t="inlineStr">
+        <is>
+          <t>3.877189e-02</t>
+        </is>
+      </c>
+      <c r="BT23" t="inlineStr">
+        <is>
+          <t>7.412202e-01</t>
+        </is>
+      </c>
+      <c r="BU23" t="inlineStr">
+        <is>
+          <t>1.553267e+00</t>
+        </is>
+      </c>
+      <c r="BV23" t="inlineStr">
+        <is>
+          <t>3.280110e+01</t>
+        </is>
+      </c>
+      <c r="BW23" t="inlineStr">
+        <is>
+          <t>5.347686e+00</t>
+        </is>
+      </c>
+      <c r="BX23" t="inlineStr">
+        <is>
+          <t>4.184313e-02</t>
+        </is>
+      </c>
+      <c r="BY23" t="inlineStr">
+        <is>
+          <t>-1.586914e+00</t>
+        </is>
+      </c>
+      <c r="BZ23" t="inlineStr">
+        <is>
+          <t>2.521799e+03</t>
+        </is>
+      </c>
+      <c r="CA23" t="inlineStr">
+        <is>
+          <t>4.419523e-01</t>
+        </is>
+      </c>
+      <c r="CB23" t="inlineStr">
+        <is>
+          <t>2.441406e-01</t>
+        </is>
+      </c>
+      <c r="CC23" t="inlineStr">
+        <is>
+          <t>2.927613e-02</t>
+        </is>
+      </c>
+      <c r="CD23" t="inlineStr">
+        <is>
+          <t>5.464355e-02</t>
+        </is>
+      </c>
+      <c r="CE23" t="inlineStr">
+        <is>
+          <t>-5.644368e-02</t>
+        </is>
+      </c>
+      <c r="CF23" t="inlineStr">
+        <is>
+          <t>-9.587158e-03</t>
+        </is>
+      </c>
+      <c r="CG23" t="inlineStr">
+        <is>
+          <t>5.147709e+00</t>
+        </is>
+      </c>
+      <c r="CH23" t="inlineStr">
+        <is>
+          <t>4.920354e+00</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
           <t>LWP758</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>7.647991e+00</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="F24" t="inlineStr">
         <is>
           <t>1.217171e+00</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
+      <c r="G24" t="inlineStr">
         <is>
           <t>7.237035e+00</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr">
+      <c r="H24" t="inlineStr">
         <is>
           <t>1.974221e+01</t>
         </is>
       </c>
-      <c r="I23" t="inlineStr">
+      <c r="I24" t="inlineStr">
         <is>
           <t>4.281611e+00</t>
         </is>
       </c>
-      <c r="J23" t="inlineStr">
+      <c r="J24" t="inlineStr">
         <is>
           <t>3.616100e+00</t>
         </is>
       </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>0.000000e+00</t>
-        </is>
-      </c>
-      <c r="L23" t="inlineStr">
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>0.000000e+00</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
         <is>
           <t>1.046911e+01</t>
         </is>
       </c>
-      <c r="M23" t="inlineStr">
+      <c r="M24" t="inlineStr">
         <is>
           <t>1.222028e+01</t>
         </is>
       </c>
-      <c r="N23" t="inlineStr">
+      <c r="N24" t="inlineStr">
         <is>
           <t>7.120622e+00</t>
         </is>
       </c>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>0.000000e+00</t>
-        </is>
-      </c>
-      <c r="P23" t="inlineStr">
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>0.000000e+00</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
         <is>
           <t>5.252108e+00</t>
         </is>
       </c>
-      <c r="Q23" t="inlineStr">
+      <c r="Q24" t="inlineStr">
         <is>
           <t>1.549001e+01</t>
         </is>
       </c>
-      <c r="R23" t="inlineStr">
+      <c r="R24" t="inlineStr">
         <is>
           <t>9.250815e+00</t>
         </is>
       </c>
-      <c r="S23" t="inlineStr">
+      <c r="S24" t="inlineStr">
         <is>
           <t>6.931388e+00</t>
         </is>
       </c>
-      <c r="T23" t="inlineStr">
-        <is>
-          <t>0.000000e+00</t>
-        </is>
-      </c>
-      <c r="U23" t="inlineStr">
+      <c r="T24" t="inlineStr">
+        <is>
+          <t>0.000000e+00</t>
+        </is>
+      </c>
+      <c r="U24" t="inlineStr">
         <is>
           <t>1.525038e+00</t>
         </is>
       </c>
-      <c r="V23" t="inlineStr">
+      <c r="V24" t="inlineStr">
         <is>
           <t>1.073994e+01</t>
         </is>
       </c>
-      <c r="W23" t="inlineStr">
+      <c r="W24" t="inlineStr">
         <is>
           <t>3.621569e+00</t>
         </is>
       </c>
-      <c r="X23" t="inlineStr">
+      <c r="X24" t="inlineStr">
         <is>
           <t>2.474082e+01</t>
         </is>
       </c>
-      <c r="Y23" t="inlineStr">
+      <c r="Y24" t="inlineStr">
         <is>
           <t>1.054749e+01</t>
         </is>
       </c>
-      <c r="Z23" t="inlineStr">
+      <c r="Z24" t="inlineStr">
         <is>
           <t>2.268940e+01</t>
         </is>
       </c>
-      <c r="AA23" t="inlineStr">
+      <c r="AA24" t="inlineStr">
         <is>
           <t>LWP758</t>
         </is>
       </c>
-      <c r="AB23" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="AC23" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="AD23" t="inlineStr">
+      <c r="AB24" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="AC24" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="AD24" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="AE23" t="inlineStr">
+      <c r="AE24" t="inlineStr">
         <is>
           <t>3.245176e+00</t>
         </is>
       </c>
-      <c r="AF23" t="inlineStr">
+      <c r="AF24" t="inlineStr">
         <is>
           <t>2.087482e+00</t>
         </is>
       </c>
-      <c r="AG23" t="inlineStr">
+      <c r="AG24" t="inlineStr">
         <is>
           <t>7.136637e+00</t>
         </is>
       </c>
-      <c r="AH23" t="inlineStr">
+      <c r="AH24" t="inlineStr">
         <is>
           <t>2.210137e+00</t>
         </is>
       </c>
-      <c r="AI23" t="inlineStr">
+      <c r="AI24" t="inlineStr">
         <is>
           <t>6.634073e+00</t>
         </is>
       </c>
-      <c r="AJ23" t="inlineStr">
+      <c r="AJ24" t="inlineStr">
         <is>
           <t>3.206725e+00</t>
         </is>
       </c>
-      <c r="AK23" t="inlineStr">
+      <c r="AK24" t="inlineStr">
         <is>
           <t>3.321025e+00</t>
         </is>
       </c>
-      <c r="AL23" t="inlineStr">
+      <c r="AL24" t="inlineStr">
         <is>
           <t>7.975593e+00</t>
         </is>
       </c>
-      <c r="AM23" t="inlineStr">
+      <c r="AM24" t="inlineStr">
         <is>
           <t>5.856856e+00</t>
         </is>
       </c>
-      <c r="AN23" t="inlineStr">
+      <c r="AN24" t="inlineStr">
         <is>
           <t>3.586366e+00</t>
         </is>
       </c>
-      <c r="AO23" t="inlineStr">
+      <c r="AO24" t="inlineStr">
         <is>
           <t>3.826889e+00</t>
         </is>
       </c>
-      <c r="AP23" t="inlineStr">
+      <c r="AP24" t="inlineStr">
         <is>
           <t>3.122414e+00</t>
         </is>
       </c>
-      <c r="AQ23" t="inlineStr">
+      <c r="AQ24" t="inlineStr">
         <is>
           <t>4.263797e+00</t>
         </is>
       </c>
-      <c r="AR23" t="inlineStr">
+      <c r="AR24" t="inlineStr">
         <is>
           <t>5.489644e+00</t>
         </is>
       </c>
-      <c r="AS23" t="inlineStr">
+      <c r="AS24" t="inlineStr">
         <is>
           <t>2.722585e+00</t>
         </is>
       </c>
-      <c r="AT23" t="inlineStr">
+      <c r="AT24" t="inlineStr">
         <is>
           <t>9.076109e-01</t>
         </is>
       </c>
-      <c r="AU23" t="inlineStr">
+      <c r="AU24" t="inlineStr">
         <is>
           <t>1.158232e+00</t>
         </is>
       </c>
-      <c r="AV23" t="inlineStr">
+      <c r="AV24" t="inlineStr">
         <is>
           <t>6.309373e+00</t>
         </is>
       </c>
-      <c r="AW23" t="inlineStr">
+      <c r="AW24" t="inlineStr">
         <is>
           <t>2.372040e+00</t>
         </is>
       </c>
-      <c r="AX23" t="inlineStr">
+      <c r="AX24" t="inlineStr">
         <is>
           <t>2.264586e+00</t>
         </is>
       </c>
-      <c r="AY23" t="inlineStr">
+      <c r="AY24" t="inlineStr">
         <is>
           <t>1.003864e+00</t>
         </is>
       </c>
-      <c r="AZ23" t="inlineStr">
+      <c r="AZ24" t="inlineStr">
         <is>
           <t>8.736255e+00</t>
         </is>
       </c>
-      <c r="BA23" t="inlineStr">
+      <c r="BA24" t="inlineStr">
         <is>
           <t>LWP758</t>
         </is>
       </c>
-      <c r="BB23" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="BC23" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="BD23" t="inlineStr">
+      <c r="BB24" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="BC24" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="BD24" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="BE23" t="inlineStr">
+      <c r="BE24" t="inlineStr">
         <is>
           <t>1.207545e+00</t>
         </is>
       </c>
-      <c r="BF23" t="inlineStr">
+      <c r="BF24" t="inlineStr">
         <is>
           <t>2.433514e+01</t>
         </is>
       </c>
-      <c r="BG23" t="inlineStr">
+      <c r="BG24" t="inlineStr">
         <is>
           <t>9.590888e+01</t>
         </is>
       </c>
-      <c r="BH23" t="inlineStr">
-        <is>
-          <t>0.000000e+00</t>
-        </is>
-      </c>
-      <c r="BI23" t="inlineStr">
+      <c r="BH24" t="inlineStr">
+        <is>
+          <t>0.000000e+00</t>
+        </is>
+      </c>
+      <c r="BI24" t="inlineStr">
         <is>
           <t>4.202680e-02</t>
         </is>
       </c>
-      <c r="BJ23" t="inlineStr">
+      <c r="BJ24" t="inlineStr">
         <is>
           <t>5.371094e+00</t>
         </is>
       </c>
-      <c r="BK23" t="inlineStr">
+      <c r="BK24" t="inlineStr">
         <is>
           <t>7.020637e+00</t>
         </is>
       </c>
-      <c r="BL23" t="inlineStr">
+      <c r="BL24" t="inlineStr">
         <is>
           <t>8.477733e+00</t>
         </is>
       </c>
-      <c r="BM23" t="inlineStr">
+      <c r="BM24" t="inlineStr">
         <is>
           <t>8.477733e+00</t>
         </is>
       </c>
-      <c r="BN23" t="inlineStr">
+      <c r="BN24" t="inlineStr">
         <is>
           <t>1.236412e-02</t>
         </is>
       </c>
-      <c r="BO23" t="inlineStr">
+      <c r="BO24" t="inlineStr">
         <is>
           <t>1.194178e-02</t>
         </is>
       </c>
-      <c r="BP23" t="inlineStr">
+      <c r="BP24" t="inlineStr">
         <is>
           <t>4.650955e+00</t>
         </is>
       </c>
-      <c r="BQ23" t="inlineStr">
+      <c r="BQ24" t="inlineStr">
         <is>
           <t>1.673508e+01</t>
         </is>
       </c>
-      <c r="BR23" t="inlineStr">
+      <c r="BR24" t="inlineStr">
         <is>
           <t>6.515555e+01</t>
         </is>
       </c>
-      <c r="BS23" t="inlineStr">
+      <c r="BS24" t="inlineStr">
         <is>
           <t>3.347589e-02</t>
         </is>
       </c>
-      <c r="BT23" t="inlineStr">
+      <c r="BT24" t="inlineStr">
         <is>
           <t>-3.779603e+01</t>
         </is>
       </c>
-      <c r="BU23" t="inlineStr">
+      <c r="BU24" t="inlineStr">
         <is>
           <t>-9.397741e+00</t>
         </is>
       </c>
-      <c r="BV23" t="inlineStr">
+      <c r="BV24" t="inlineStr">
         <is>
           <t>2.972641e+01</t>
         </is>
       </c>
-      <c r="BW23" t="inlineStr">
+      <c r="BW24" t="inlineStr">
         <is>
           <t>7.579457e+00</t>
         </is>
       </c>
-      <c r="BX23" t="inlineStr">
+      <c r="BX24" t="inlineStr">
         <is>
           <t>5.930642e-02</t>
         </is>
       </c>
-      <c r="BY23" t="inlineStr">
+      <c r="BY24" t="inlineStr">
         <is>
           <t>1.464844e+00</t>
         </is>
       </c>
-      <c r="BZ23" t="inlineStr">
+      <c r="BZ24" t="inlineStr">
         <is>
           <t>2.489279e+03</t>
         </is>
       </c>
-      <c r="CA23" t="inlineStr">
+      <c r="CA24" t="inlineStr">
         <is>
           <t>1.845296e-01</t>
         </is>
       </c>
-      <c r="CB23" t="inlineStr">
+      <c r="CB24" t="inlineStr">
         <is>
           <t>1.342773e+00</t>
         </is>
       </c>
-      <c r="CC23" t="inlineStr">
+      <c r="CC24" t="inlineStr">
         <is>
           <t>1.872792e-02</t>
         </is>
       </c>
-      <c r="CD23" t="inlineStr">
+      <c r="CD24" t="inlineStr">
         <is>
           <t>3.471696e-02</t>
         </is>
       </c>
-      <c r="CE23" t="inlineStr">
+      <c r="CE24" t="inlineStr">
         <is>
           <t>-3.585251e-02</t>
         </is>
       </c>
-      <c r="CF23" t="inlineStr">
+      <c r="CF24" t="inlineStr">
         <is>
           <t>1.632873e-03</t>
         </is>
       </c>
-      <c r="CG23" t="inlineStr">
+      <c r="CG24" t="inlineStr">
         <is>
           <t>5.336861e+00</t>
         </is>
       </c>
-      <c r="CH23" t="inlineStr">
+      <c r="CH24" t="inlineStr">
         <is>
           <t>4.519424e+00</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>LWP759</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>5.451049e+00</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>9.502499e-01</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>8.497318e+00</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>1.313842e+01</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>0.000000e+00</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>4.204835e+00</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>0.000000e+00</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>6.382168e+00</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>9.544452e+00</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>4.931680e+00</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>0.000000e+00</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>4.588327e+00</t>
+        </is>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>3.041443e+00</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>7.694183e+00</t>
+        </is>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>3.292280e+00</t>
+        </is>
+      </c>
+      <c r="T25" t="inlineStr">
+        <is>
+          <t>0.000000e+00</t>
+        </is>
+      </c>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>0.000000e+00</t>
+        </is>
+      </c>
+      <c r="V25" t="inlineStr">
+        <is>
+          <t>4.935686e+00</t>
+        </is>
+      </c>
+      <c r="W25" t="inlineStr">
+        <is>
+          <t>1.173626e+01</t>
+        </is>
+      </c>
+      <c r="X25" t="inlineStr">
+        <is>
+          <t>1.073563e+01</t>
+        </is>
+      </c>
+      <c r="Y25" t="inlineStr">
+        <is>
+          <t>7.497115e+00</t>
+        </is>
+      </c>
+      <c r="Z25" t="inlineStr">
+        <is>
+          <t>1.592662e+01</t>
+        </is>
+      </c>
+      <c r="AA25" t="inlineStr">
+        <is>
+          <t>LWP759</t>
+        </is>
+      </c>
+      <c r="AB25" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="AC25" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="AD25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AE25" t="inlineStr">
+        <is>
+          <t>3.653519e+00</t>
+        </is>
+      </c>
+      <c r="AF25" t="inlineStr">
+        <is>
+          <t>3.110123e+00</t>
+        </is>
+      </c>
+      <c r="AG25" t="inlineStr">
+        <is>
+          <t>7.685993e+00</t>
+        </is>
+      </c>
+      <c r="AH25" t="inlineStr">
+        <is>
+          <t>2.617976e+00</t>
+        </is>
+      </c>
+      <c r="AI25" t="inlineStr">
+        <is>
+          <t>3.323220e+00</t>
+        </is>
+      </c>
+      <c r="AJ25" t="inlineStr">
+        <is>
+          <t>3.525192e+00</t>
+        </is>
+      </c>
+      <c r="AK25" t="inlineStr">
+        <is>
+          <t>3.489393e+00</t>
+        </is>
+      </c>
+      <c r="AL25" t="inlineStr">
+        <is>
+          <t>9.964922e+00</t>
+        </is>
+      </c>
+      <c r="AM25" t="inlineStr">
+        <is>
+          <t>5.406873e+00</t>
+        </is>
+      </c>
+      <c r="AN25" t="inlineStr">
+        <is>
+          <t>3.832273e+00</t>
+        </is>
+      </c>
+      <c r="AO25" t="inlineStr">
+        <is>
+          <t>5.456108e+00</t>
+        </is>
+      </c>
+      <c r="AP25" t="inlineStr">
+        <is>
+          <t>5.296775e+00</t>
+        </is>
+      </c>
+      <c r="AQ25" t="inlineStr">
+        <is>
+          <t>3.629478e+00</t>
+        </is>
+      </c>
+      <c r="AR25" t="inlineStr">
+        <is>
+          <t>4.189168e+00</t>
+        </is>
+      </c>
+      <c r="AS25" t="inlineStr">
+        <is>
+          <t>2.958365e+00</t>
+        </is>
+      </c>
+      <c r="AT25" t="inlineStr">
+        <is>
+          <t>1.045301e+00</t>
+        </is>
+      </c>
+      <c r="AU25" t="inlineStr">
+        <is>
+          <t>7.048995e-01</t>
+        </is>
+      </c>
+      <c r="AV25" t="inlineStr">
+        <is>
+          <t>7.078426e+00</t>
+        </is>
+      </c>
+      <c r="AW25" t="inlineStr">
+        <is>
+          <t>7.123482e+00</t>
+        </is>
+      </c>
+      <c r="AX25" t="inlineStr">
+        <is>
+          <t>2.244263e+00</t>
+        </is>
+      </c>
+      <c r="AY25" t="inlineStr">
+        <is>
+          <t>1.047139e+00</t>
+        </is>
+      </c>
+      <c r="AZ25" t="inlineStr">
+        <is>
+          <t>7.837752e+00</t>
+        </is>
+      </c>
+      <c r="BA25" t="inlineStr">
+        <is>
+          <t>LWP759</t>
+        </is>
+      </c>
+      <c r="BB25" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="BC25" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="BD25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BE25" t="inlineStr">
+        <is>
+          <t>1.274552e+00</t>
+        </is>
+      </c>
+      <c r="BF25" t="inlineStr">
+        <is>
+          <t>3.949726e+01</t>
+        </is>
+      </c>
+      <c r="BG25" t="inlineStr">
+        <is>
+          <t>9.262039e+01</t>
+        </is>
+      </c>
+      <c r="BH25" t="inlineStr">
+        <is>
+          <t>0.000000e+00</t>
+        </is>
+      </c>
+      <c r="BI25" t="inlineStr">
+        <is>
+          <t>5.730891e-02</t>
+        </is>
+      </c>
+      <c r="BJ25" t="inlineStr">
+        <is>
+          <t>7.324219e+00</t>
+        </is>
+      </c>
+      <c r="BK25" t="inlineStr">
+        <is>
+          <t>4.351481e+00</t>
+        </is>
+      </c>
+      <c r="BL25" t="inlineStr">
+        <is>
+          <t>5.546189e+00</t>
+        </is>
+      </c>
+      <c r="BM25" t="inlineStr">
+        <is>
+          <t>5.546189e+00</t>
+        </is>
+      </c>
+      <c r="BN25" t="inlineStr">
+        <is>
+          <t>1.342740e-02</t>
+        </is>
+      </c>
+      <c r="BO25" t="inlineStr">
+        <is>
+          <t>1.420914e-02</t>
+        </is>
+      </c>
+      <c r="BP25" t="inlineStr">
+        <is>
+          <t>4.650955e+00</t>
+        </is>
+      </c>
+      <c r="BQ25" t="inlineStr">
+        <is>
+          <t>1.000000e+00</t>
+        </is>
+      </c>
+      <c r="BR25" t="inlineStr">
+        <is>
+          <t>6.401307e+01</t>
+        </is>
+      </c>
+      <c r="BS25" t="inlineStr">
+        <is>
+          <t>3.318089e-02</t>
+        </is>
+      </c>
+      <c r="BT25" t="inlineStr">
+        <is>
+          <t>-4.013775e+01</t>
+        </is>
+      </c>
+      <c r="BU25" t="inlineStr">
+        <is>
+          <t>-1.053494e+01</t>
+        </is>
+      </c>
+      <c r="BV25" t="inlineStr">
+        <is>
+          <t>2.973154e+01</t>
+        </is>
+      </c>
+      <c r="BW25" t="inlineStr">
+        <is>
+          <t>7.528649e+00</t>
+        </is>
+      </c>
+      <c r="BX25" t="inlineStr">
+        <is>
+          <t>5.890849e-02</t>
+        </is>
+      </c>
+      <c r="BY25" t="inlineStr">
+        <is>
+          <t>1.953125e+00</t>
+        </is>
+      </c>
+      <c r="BZ25" t="inlineStr">
+        <is>
+          <t>2.092423e+03</t>
+        </is>
+      </c>
+      <c r="CA25" t="inlineStr">
+        <is>
+          <t>3.736927e-02</t>
+        </is>
+      </c>
+      <c r="CB25" t="inlineStr">
+        <is>
+          <t>-1.464844e+00</t>
+        </is>
+      </c>
+      <c r="CC25" t="inlineStr">
+        <is>
+          <t>2.391154e-02</t>
+        </is>
+      </c>
+      <c r="CD25" t="inlineStr">
+        <is>
+          <t>3.567221e-02</t>
+        </is>
+      </c>
+      <c r="CE25" t="inlineStr">
+        <is>
+          <t>-5.811827e-02</t>
+        </is>
+      </c>
+      <c r="CF25" t="inlineStr">
+        <is>
+          <t>-1.101613e-02</t>
+        </is>
+      </c>
+      <c r="CG25" t="inlineStr">
+        <is>
+          <t>7.017213e+00</t>
+        </is>
+      </c>
+      <c r="CH25" t="inlineStr">
+        <is>
+          <t>6.135004e+00</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>LWP761</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>6.118854e+00</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>3.014558e+00</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>1.123057e+01</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>1.343019e+01</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>1.770977e+01</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>3.411086e+00</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>1.312506e+01</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>1.331110e+01</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>0.000000e+00</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>4.780475e+00</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>0.000000e+00</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>9.262909e+00</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>1.429085e+01</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>5.009841e+00</t>
+        </is>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>4.830960e+00</t>
+        </is>
+      </c>
+      <c r="T26" t="inlineStr">
+        <is>
+          <t>0.000000e+00</t>
+        </is>
+      </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>0.000000e+00</t>
+        </is>
+      </c>
+      <c r="V26" t="inlineStr">
+        <is>
+          <t>5.105047e+00</t>
+        </is>
+      </c>
+      <c r="W26" t="inlineStr">
+        <is>
+          <t>2.525332e+00</t>
+        </is>
+      </c>
+      <c r="X26" t="inlineStr">
+        <is>
+          <t>1.930069e+01</t>
+        </is>
+      </c>
+      <c r="Y26" t="inlineStr">
+        <is>
+          <t>8.242046e+00</t>
+        </is>
+      </c>
+      <c r="Z26" t="inlineStr">
+        <is>
+          <t>1.331110e+01</t>
+        </is>
+      </c>
+      <c r="AA26" t="inlineStr">
+        <is>
+          <t>LWP761</t>
+        </is>
+      </c>
+      <c r="AB26" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="AC26" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="AD26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AE26" t="inlineStr">
+        <is>
+          <t>2.411602e+00</t>
+        </is>
+      </c>
+      <c r="AF26" t="inlineStr">
+        <is>
+          <t>2.311945e+00</t>
+        </is>
+      </c>
+      <c r="AG26" t="inlineStr">
+        <is>
+          <t>7.189678e+00</t>
+        </is>
+      </c>
+      <c r="AH26" t="inlineStr">
+        <is>
+          <t>1.525735e+00</t>
+        </is>
+      </c>
+      <c r="AI26" t="inlineStr">
+        <is>
+          <t>4.649536e+00</t>
+        </is>
+      </c>
+      <c r="AJ26" t="inlineStr">
+        <is>
+          <t>2.325064e+00</t>
+        </is>
+      </c>
+      <c r="AK26" t="inlineStr">
+        <is>
+          <t>5.342087e+00</t>
+        </is>
+      </c>
+      <c r="AL26" t="inlineStr">
+        <is>
+          <t>5.518427e+00</t>
+        </is>
+      </c>
+      <c r="AM26" t="inlineStr">
+        <is>
+          <t>2.841814e+00</t>
+        </is>
+      </c>
+      <c r="AN26" t="inlineStr">
+        <is>
+          <t>3.028984e+00</t>
+        </is>
+      </c>
+      <c r="AO26" t="inlineStr">
+        <is>
+          <t>4.161012e+00</t>
+        </is>
+      </c>
+      <c r="AP26" t="inlineStr">
+        <is>
+          <t>4.152146e+00</t>
+        </is>
+      </c>
+      <c r="AQ26" t="inlineStr">
+        <is>
+          <t>2.792679e+00</t>
+        </is>
+      </c>
+      <c r="AR26" t="inlineStr">
+        <is>
+          <t>3.843069e+00</t>
+        </is>
+      </c>
+      <c r="AS26" t="inlineStr">
+        <is>
+          <t>2.497338e+00</t>
+        </is>
+      </c>
+      <c r="AT26" t="inlineStr">
+        <is>
+          <t>7.317323e-01</t>
+        </is>
+      </c>
+      <c r="AU26" t="inlineStr">
+        <is>
+          <t>3.837709e-01</t>
+        </is>
+      </c>
+      <c r="AV26" t="inlineStr">
+        <is>
+          <t>3.419148e+00</t>
+        </is>
+      </c>
+      <c r="AW26" t="inlineStr">
+        <is>
+          <t>4.669459e+00</t>
+        </is>
+      </c>
+      <c r="AX26" t="inlineStr">
+        <is>
+          <t>1.718610e+00</t>
+        </is>
+      </c>
+      <c r="AY26" t="inlineStr">
+        <is>
+          <t>6.346550e-01</t>
+        </is>
+      </c>
+      <c r="AZ26" t="inlineStr">
+        <is>
+          <t>5.471623e+00</t>
+        </is>
+      </c>
+      <c r="BA26" t="inlineStr">
+        <is>
+          <t>LWP761</t>
+        </is>
+      </c>
+      <c r="BB26" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="BC26" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="BD26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BE26" t="inlineStr">
+        <is>
+          <t>1.263432e+00</t>
+        </is>
+      </c>
+      <c r="BF26" t="inlineStr">
+        <is>
+          <t>2.235105e+01</t>
+        </is>
+      </c>
+      <c r="BG26" t="inlineStr">
+        <is>
+          <t>9.087173e+01</t>
+        </is>
+      </c>
+      <c r="BH26" t="inlineStr">
+        <is>
+          <t>0.000000e+00</t>
+        </is>
+      </c>
+      <c r="BI26" t="inlineStr">
+        <is>
+          <t>3.438524e-02</t>
+        </is>
+      </c>
+      <c r="BJ26" t="inlineStr">
+        <is>
+          <t>4.394531e+00</t>
+        </is>
+      </c>
+      <c r="BK26" t="inlineStr">
+        <is>
+          <t>7.241522e+00</t>
+        </is>
+      </c>
+      <c r="BL26" t="inlineStr">
+        <is>
+          <t>9.149173e+00</t>
+        </is>
+      </c>
+      <c r="BM26" t="inlineStr">
+        <is>
+          <t>9.149173e+00</t>
+        </is>
+      </c>
+      <c r="BN26" t="inlineStr">
+        <is>
+          <t>9.962855e-03</t>
+        </is>
+      </c>
+      <c r="BO26" t="inlineStr">
+        <is>
+          <t>1.055196e-02</t>
+        </is>
+      </c>
+      <c r="BP26" t="inlineStr">
+        <is>
+          <t>4.660507e+00</t>
+        </is>
+      </c>
+      <c r="BQ26" t="inlineStr">
+        <is>
+          <t>3.338803e+01</t>
+        </is>
+      </c>
+      <c r="BR26" t="inlineStr">
+        <is>
+          <t>4.068426e+01</t>
+        </is>
+      </c>
+      <c r="BS26" t="inlineStr">
+        <is>
+          <t>2.645243e-02</t>
+        </is>
+      </c>
+      <c r="BT26" t="inlineStr">
+        <is>
+          <t>-4.213503e+00</t>
+        </is>
+      </c>
+      <c r="BU26" t="inlineStr">
+        <is>
+          <t>6.112170e+00</t>
+        </is>
+      </c>
+      <c r="BV26" t="inlineStr">
+        <is>
+          <t>2.955487e+01</t>
+        </is>
+      </c>
+      <c r="BW26" t="inlineStr">
+        <is>
+          <t>7.052790e+00</t>
+        </is>
+      </c>
+      <c r="BX26" t="inlineStr">
+        <is>
+          <t>5.518493e-02</t>
+        </is>
+      </c>
+      <c r="BY26" t="inlineStr">
+        <is>
+          <t>9.765625e-01</t>
+        </is>
+      </c>
+      <c r="BZ26" t="inlineStr">
+        <is>
+          <t>2.800889e+03</t>
+        </is>
+      </c>
+      <c r="CA26" t="inlineStr">
+        <is>
+          <t>2.781359e-01</t>
+        </is>
+      </c>
+      <c r="CB26" t="inlineStr">
+        <is>
+          <t>1.953125e+00</t>
+        </is>
+      </c>
+      <c r="CC26" t="inlineStr">
+        <is>
+          <t>1.415042e-02</t>
+        </is>
+      </c>
+      <c r="CD26" t="inlineStr">
+        <is>
+          <t>3.334129e-02</t>
+        </is>
+      </c>
+      <c r="CE26" t="inlineStr">
+        <is>
+          <t>-3.007996e-02</t>
+        </is>
+      </c>
+      <c r="CF26" t="inlineStr">
+        <is>
+          <t>8.295887e-04</t>
+        </is>
+      </c>
+      <c r="CG26" t="inlineStr">
+        <is>
+          <t>4.848904e+00</t>
+        </is>
+      </c>
+      <c r="CH26" t="inlineStr">
+        <is>
+          <t>4.443189e+00</t>
         </is>
       </c>
     </row>

</xml_diff>